<commit_message>
Desafios 9, 10 e 11
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\potew\GitHub\Projetos\B22-MySQL-One-for-All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2130DBDB-B009-4BC4-B33F-3B70BE2DAB15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09A03E8-3C28-4E0D-A603-389783C4CA79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="2475" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -241,7 +241,7 @@
     <t>Subscription_plans</t>
   </si>
   <si>
-    <t>Track_play</t>
+    <t>Track_history</t>
   </si>
 </sst>
 </file>
@@ -664,6 +664,82 @@
   <dxfs count="44">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1072,82 +1148,6 @@
           <color indexed="11"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1354,10 +1354,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4C22B1FD-AAB4-4572-947D-B9AA26FF4CA6}" name="Tabela2" displayName="Tabela2" ref="G3:G6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="21" headerRowBorderDxfId="42" tableBorderDxfId="43" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4C22B1FD-AAB4-4572-947D-B9AA26FF4CA6}" name="Tabela2" displayName="Tabela2" ref="G3:G6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="25" headerRowBorderDxfId="42" tableBorderDxfId="43" totalsRowBorderDxfId="41">
   <autoFilter ref="G3:G6" xr:uid="{7135D481-8CAC-445D-A87B-90BBD089606F}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{F534BE95-1E1C-4506-B6D3-9F0EA128A7F8}" name="id" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{F534BE95-1E1C-4506-B6D3-9F0EA128A7F8}" name="id" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1376,62 +1376,62 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9E64903A-209B-4BB8-A204-543F9417B011}" name="Tabela5" displayName="Tabela5" ref="B18:D36" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9E64903A-209B-4BB8-A204-543F9417B011}" name="Tabela5" displayName="Tabela5" ref="B18:D36" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="B18:D36" xr:uid="{10ED3BF6-1F70-4901-B2B6-2BBCE8C1A970}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B19:D34">
     <sortCondition ref="B18:B34"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D1BAADAB-FE74-47D0-A135-34D923F403A4}" name="id" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{CBC7B815-F679-4613-AB1C-FEE233FAFCB5}" name="song_name" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{F06A1B0F-F08F-4280-B6E7-8086ECEF1830}" name="album_id" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{D1BAADAB-FE74-47D0-A135-34D923F403A4}" name="id" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{CBC7B815-F679-4613-AB1C-FEE233FAFCB5}" name="song_name" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{F06A1B0F-F08F-4280-B6E7-8086ECEF1830}" name="album_id" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0D4CCA0F-99E7-4733-8F3A-5225F4914434}" name="Tabela6" displayName="Tabela6" ref="K20:M28" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0D4CCA0F-99E7-4733-8F3A-5225F4914434}" name="Tabela6" displayName="Tabela6" ref="K20:M28" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="K20:M28" xr:uid="{E7BF67C9-1F06-4C85-A880-E3AD420CF756}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BC745BBB-72BA-418C-B4AB-674D1363F616}" name="id" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{165B1ACB-5035-440D-892F-9E263C1BD6CB}" name="user_id" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{65496510-4D50-4191-8D65-4CD53DE8087D}" name="artist_id" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{BC745BBB-72BA-418C-B4AB-674D1363F616}" name="id" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{165B1ACB-5035-440D-892F-9E263C1BD6CB}" name="user_id" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{65496510-4D50-4191-8D65-4CD53DE8087D}" name="artist_id" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5C4DD743-3EED-4221-B999-48AFCB76BECF}" name="Tabela7" displayName="Tabela7" ref="G9:H13" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5C4DD743-3EED-4221-B999-48AFCB76BECF}" name="Tabela7" displayName="Tabela7" ref="G9:H13" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="G9:H13" xr:uid="{8A6A4E10-412A-46D0-BC0B-9A701AB4D756}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1B482CE1-2F00-44A1-97E9-A845D9A7EE9F}" name="id" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{80AD9FDC-83D1-49A1-A765-9B1CD077F957}" name="artist_name" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{1B482CE1-2F00-44A1-97E9-A845D9A7EE9F}" name="id" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{80AD9FDC-83D1-49A1-A765-9B1CD077F957}" name="artist_name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3F44D105-5037-42DA-8441-90D92BEC1473}" name="Tabela8" displayName="Tabela8" ref="G15:H19" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="27" tableBorderDxfId="28" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3F44D105-5037-42DA-8441-90D92BEC1473}" name="Tabela8" displayName="Tabela8" ref="G15:H19" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowBorderDxfId="31" tableBorderDxfId="32" totalsRowBorderDxfId="30">
   <autoFilter ref="G15:H19" xr:uid="{E9AAE537-CDF5-4F8B-B90C-7DF145DED496}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{264A3B82-55A9-4BEF-BF49-4693C85E4C56}" name="usuario_id" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{61798E3C-602C-4E38-8C5B-21DDB9B2D223}" name="seguindo_artistas" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{264A3B82-55A9-4BEF-BF49-4693C85E4C56}" name="usuario_id" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{61798E3C-602C-4E38-8C5B-21DDB9B2D223}" name="seguindo_artistas" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{34969B50-8BC9-4609-B07E-D8E5882DAA62}" name="Tabela9" displayName="Tabela9" ref="B3:E7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13" headerRowBorderDxfId="19" tableBorderDxfId="20" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{34969B50-8BC9-4609-B07E-D8E5882DAA62}" name="Tabela9" displayName="Tabela9" ref="B3:E7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="17" headerRowBorderDxfId="23" tableBorderDxfId="24" totalsRowBorderDxfId="22">
   <autoFilter ref="B3:E7" xr:uid="{ACF26A9D-1225-4365-AD0D-40E29CA03B14}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B90A6C15-19D4-4B8F-8E2C-0A5738AE4EF5}" name="id" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{EFFF63C5-D547-44C6-99AB-31345A850905}" name="user_name" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{82C7822E-1330-4EFC-8B70-4FB847B1B823}" name="user_age" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{713782BB-CA29-44B6-BAF1-0FEEDF3D87B6}" name="plan_id" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{B90A6C15-19D4-4B8F-8E2C-0A5738AE4EF5}" name="id" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{EFFF63C5-D547-44C6-99AB-31345A850905}" name="user_name" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{82C7822E-1330-4EFC-8B70-4FB847B1B823}" name="user_age" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{713782BB-CA29-44B6-BAF1-0FEEDF3D87B6}" name="plan_id" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2515,7 +2515,7 @@
   <dimension ref="B1:M36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2524,7 +2524,7 @@
     <col min="2" max="2" width="22.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="5.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.44140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.21875" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
Typo in artist name
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\potew\GitHub\Projetos\B22-MySQL-One-for-All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7436A7-FCAF-4126-9474-65DE239D959B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1463855-7FFF-4140-B057-B871964D014B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
   <si>
     <t>usuario_id</t>
   </si>
@@ -214,7 +214,10 @@
     <t>Track_history</t>
   </si>
   <si>
-    <t>PRIMARY KEY (user_id, artist_id)</t>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>(user_id, artist_id)</t>
   </si>
 </sst>
 </file>
@@ -282,7 +285,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -524,6 +527,21 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -555,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -667,15 +685,17 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2510,7 +2530,7 @@
   <dimension ref="B1:M36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2566,7 +2586,7 @@
       <c r="I3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="45" t="s">
         <v>64</v>
       </c>
       <c r="L3" s="4" t="s">
@@ -2599,7 +2619,9 @@
       <c r="I4" s="18">
         <v>0</v>
       </c>
-      <c r="K4" s="42"/>
+      <c r="K4" s="41" t="s">
+        <v>65</v>
+      </c>
       <c r="L4" s="3">
         <v>1</v>
       </c>
@@ -2954,7 +2976,7 @@
       <c r="D20" s="3">
         <v>3</v>
       </c>
-      <c r="K20" s="41" t="s">
+      <c r="K20" s="44" t="s">
         <v>64</v>
       </c>
       <c r="L20" s="39" t="s">
@@ -2974,7 +2996,9 @@
       <c r="D21" s="3">
         <v>4</v>
       </c>
-      <c r="K21" s="42"/>
+      <c r="K21" s="41" t="s">
+        <v>65</v>
+      </c>
       <c r="L21" s="3">
         <v>1</v>
       </c>
@@ -3202,8 +3226,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="K3:K17"/>
-    <mergeCell ref="K20:K28"/>
+    <mergeCell ref="K4:K17"/>
+    <mergeCell ref="K21:K28"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>